<commit_message>
ECP-1107: adds adapted maintenance for turnover rent terms Sweden - now including percentage and using manual turnover rent value on regular lease term for turnover terms
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/turnover_rent_fixed_import.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/turnover_rent_fixed_import.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF8C229-9830-7743-B11C-BF254551C286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30340" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lease terms" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Lease Reference</t>
   </si>
@@ -58,12 +64,18 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Percentage Previous Year</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -143,6 +155,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -467,26 +487,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" customWidth="1"/>
+    <col min="11" max="11" width="5.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,19 +527,25 @@
         <v>11</v>
       </c>
       <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -531,20 +561,26 @@
       <c r="E2">
         <v>18000</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1">
         <v>40544</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>40908</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>21000</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2">
+        <v>6.25</v>
+      </c>
+      <c r="K2" s="3">
         <v>2011</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -560,16 +596,22 @@
       <c r="E3">
         <v>2000</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
+        <v>1.25</v>
+      </c>
+      <c r="G3" s="2">
         <v>40544</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>40908</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>2100</v>
       </c>
-      <c r="I3">
+      <c r="J3">
+        <v>1.3</v>
+      </c>
+      <c r="K3">
         <v>2011</v>
       </c>
     </row>

</xml_diff>